<commit_message>
Report into excel file
</commit_message>
<xml_diff>
--- a/src/resources/DataInput.xlsx
+++ b/src/resources/DataInput.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B97C45-6FD6-4450-B011-C8F9978989F2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environnement" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Environnement</t>
   </si>
@@ -78,20 +79,30 @@
     <t>121</t>
   </si>
   <si>
-    <t>0908608731</t>
-  </si>
-  <si>
-    <t>Hanh3091996</t>
-  </si>
-  <si>
-    <t>Login success</t>
+    <t>WebSite</t>
+  </si>
+  <si>
+    <t>https://accounts.chotot.com</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +114,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,19 +165,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -250,6 +271,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -285,6 +323,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,37 +515,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D3:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="43.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{867F98F7-0096-4C5C-93D3-2F2D9A5E09D2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select error" error="Please select an environnement in the list" promptTitle="Select the environnement">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select error" error="Please select an environnement in the list" promptTitle="Select the environnement" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Ref!$C$5:$C$7</xm:f>
           </x14:formula1>
@@ -503,97 +574,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,7 +663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C4:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -610,38 +672,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete the test without reporting with surefire
</commit_message>
<xml_diff>
--- a/src/resources/DataInput.xlsx
+++ b/src/resources/DataInput.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E633F8C-A417-4358-BF9A-C35DD0FE99B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Environnement" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Environnement</t>
   </si>
@@ -64,9 +63,6 @@
     <t>abcd</t>
   </si>
   <si>
-    <t>abc2</t>
-  </si>
-  <si>
     <t>Login failed</t>
   </si>
   <si>
@@ -76,9 +72,6 @@
     <t>1234</t>
   </si>
   <si>
-    <t>121</t>
-  </si>
-  <si>
     <t>WebSite</t>
   </si>
   <si>
@@ -88,22 +81,40 @@
     <t>Timeout</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>Login successful</t>
+  </si>
+  <si>
+    <t>0908123456</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>21654878</t>
+  </si>
+  <si>
+    <t>456487894</t>
+  </si>
+  <si>
+    <t>0907</t>
+  </si>
+  <si>
+    <t>213215468aaaa</t>
+  </si>
+  <si>
+    <t>///***</t>
+  </si>
+  <si>
+    <t>090789754</t>
+  </si>
+  <si>
+    <t>***\\\\\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,23 +284,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -325,23 +319,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,11 +494,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +514,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.25">
@@ -548,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
@@ -556,14 +533,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{867F98F7-0096-4C5C-93D3-2F2D9A5E09D2}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select error" error="Please select an environnement in the list" promptTitle="Select the environnement" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select error" error="Please select an environnement in the list" promptTitle="Select the environnement">
           <x14:formula1>
             <xm:f>Ref!$C$5:$C$7</xm:f>
           </x14:formula1>
@@ -576,11 +553,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +573,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -625,83 +602,148 @@
         <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Ref!$H$5:$H$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C4:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>